<commit_message>
sprint 2 excel and customer class
</commit_message>
<xml_diff>
--- a/Sprint 1.xlsx
+++ b/Sprint 1.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Downloads\Object Oriented\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26819"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7242"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="15080" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint NN Backlog" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint1 Backlog" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint2 Backlog" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027" fullCalcOnLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="119">
   <si>
     <t>Product Name:</t>
   </si>
@@ -322,15 +323,6 @@
     <t>RP</t>
   </si>
   <si>
-    <t>RN</t>
-  </si>
-  <si>
-    <t>RD</t>
-  </si>
-  <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>UML</t>
   </si>
   <si>
@@ -360,16 +352,46 @@
   <si>
     <t>KC and AN</t>
   </si>
+  <si>
+    <t>Create Robot Parts Classes</t>
+  </si>
+  <si>
+    <t>Create Menu</t>
+  </si>
+  <si>
+    <t>Create Product Manager Class</t>
+  </si>
+  <si>
+    <t>Create Beloved customer class</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>Update sprint 2 Backlog</t>
+  </si>
+  <si>
+    <t>backlog</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>Test Beloved Customer features</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy&quot; &quot;hh&quot;:&quot;mm&quot; &quot;AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,7 +510,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -510,6 +532,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -538,16 +561,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -562,12 +585,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="302289184"/>
-        <c:axId val="302283936"/>
+        <c:axId val="2089100328"/>
+        <c:axId val="2089092808"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="302283936"/>
+        <c:axId val="2089092808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,6 +622,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -621,12 +646,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302289184"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="2089100328"/>
+        <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="302289184"/>
+        <c:axId val="2089100328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,6 +673,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
@@ -670,8 +696,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302283936"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="2089092808"/>
+        <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -705,7 +731,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -755,28 +781,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -791,12 +817,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="361234696"/>
-        <c:axId val="361227808"/>
+        <c:axId val="2089154264"/>
+        <c:axId val="2089148328"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="361227808"/>
+        <c:axId val="2089148328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,12 +877,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361234696"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="2089154264"/>
+        <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="361234696"/>
+        <c:axId val="2089154264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -899,8 +926,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361227808"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="2089148328"/>
+        <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -934,7 +961,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -986,26 +1013,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1035,31 +1042,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F2CD-4148-860C-80E662872AB2}"/>
             </c:ext>
@@ -1073,12 +1080,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="448540176"/>
-        <c:axId val="448541816"/>
+        <c:axId val="2089208632"/>
+        <c:axId val="2089215032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448540176"/>
+        <c:axId val="2089208632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,26 +1126,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1175,7 +1163,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448541816"/>
+        <c:crossAx val="2089215032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1183,7 +1171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448541816"/>
+        <c:axId val="2089215032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,26 +1225,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1289,7 +1257,356 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448540176"/>
+        <c:crossAx val="2089208632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint2 Backlog'!$B$7:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F2CD-4148-860C-80E662872AB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2089295416"/>
+        <c:axId val="2089301816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2089295416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2089301816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2089301816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2089295416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1904,7 +2221,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD7626A8-2FAA-429B-9974-C618EAEF7137}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD7626A8-2FAA-429B-9974-C618EAEF7137}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1935,7 +2252,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01658E26-7271-4F69-AE71-FB654F51EBC8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{01658E26-7271-4F69-AE71-FB654F51EBC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1976,11 +2293,54 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C3A03C-F5B3-4980-A24B-8FA04D1E5FB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65C3A03C-F5B3-4980-A24B-8FA04D1E5FB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65C3A03C-F5B3-4980-A24B-8FA04D1E5FB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2040,7 +2400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2092,7 +2452,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2286,7 +2646,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2296,23 +2656,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.046875" customWidth="1"/>
-    <col min="2" max="2" width="4.09375" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.1875" customWidth="1"/>
-    <col min="6" max="7" width="34.47265625" customWidth="1"/>
-    <col min="8" max="8" width="56.6171875" customWidth="1"/>
-    <col min="9" max="1024" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="4.125" customWidth="1"/>
+    <col min="3" max="3" width="7.625" customWidth="1"/>
+    <col min="4" max="4" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="7.25" customWidth="1"/>
+    <col min="6" max="7" width="34.5" customWidth="1"/>
+    <col min="8" max="8" width="56.625" customWidth="1"/>
+    <col min="9" max="1024" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" ht="14.1">
+    <row r="1" spans="1:1023">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3341,7 +3701,7 @@
       <c r="AMH1" s="2"/>
       <c r="AMI1" s="2"/>
     </row>
-    <row r="2" spans="1:1023" ht="14.1">
+    <row r="2" spans="1:1023">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4368,7 +4728,7 @@
       <c r="AMH2" s="2"/>
       <c r="AMI2" s="2"/>
     </row>
-    <row r="3" spans="1:1023" ht="14.1">
+    <row r="3" spans="1:1023">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -5392,7 +5752,7 @@
       <c r="AMH3" s="2"/>
       <c r="AMI3" s="2"/>
     </row>
-    <row r="4" spans="1:1023" ht="14.1">
+    <row r="4" spans="1:1023">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -6421,7 +6781,7 @@
       <c r="AMH4" s="2"/>
       <c r="AMI4" s="2"/>
     </row>
-    <row r="5" spans="1:1023" ht="14.1">
+    <row r="5" spans="1:1023">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -7450,7 +7810,7 @@
       <c r="AMH5" s="2"/>
       <c r="AMI5" s="2"/>
     </row>
-    <row r="6" spans="1:1023" ht="14.1">
+    <row r="6" spans="1:1023">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -8479,7 +8839,7 @@
       <c r="AMH6" s="2"/>
       <c r="AMI6" s="2"/>
     </row>
-    <row r="7" spans="1:1023" ht="14.1">
+    <row r="7" spans="1:1023">
       <c r="B7" s="9"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -9503,7 +9863,7 @@
       <c r="AMH7" s="2"/>
       <c r="AMI7" s="2"/>
     </row>
-    <row r="8" spans="1:1023" ht="14.1">
+    <row r="8" spans="1:1023">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -10530,7 +10890,7 @@
       <c r="AMH8" s="2"/>
       <c r="AMI8" s="2"/>
     </row>
-    <row r="9" spans="1:1023" ht="14.1">
+    <row r="9" spans="1:1023">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -11559,7 +11919,7 @@
       <c r="AMH9" s="2"/>
       <c r="AMI9" s="2"/>
     </row>
-    <row r="10" spans="1:1023" ht="14.1">
+    <row r="10" spans="1:1023">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -12588,7 +12948,7 @@
       <c r="AMH10" s="2"/>
       <c r="AMI10" s="2"/>
     </row>
-    <row r="11" spans="1:1023" ht="14.1">
+    <row r="11" spans="1:1023">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -13617,7 +13977,7 @@
       <c r="AMH11" s="2"/>
       <c r="AMI11" s="2"/>
     </row>
-    <row r="12" spans="1:1023" ht="14.1">
+    <row r="12" spans="1:1023">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -14641,7 +15001,7 @@
       <c r="AMH12" s="2"/>
       <c r="AMI12" s="2"/>
     </row>
-    <row r="13" spans="1:1023" ht="14.1">
+    <row r="13" spans="1:1023">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -15668,7 +16028,7 @@
       <c r="AMH13" s="2"/>
       <c r="AMI13" s="2"/>
     </row>
-    <row r="14" spans="1:1023" ht="14.1">
+    <row r="14" spans="1:1023">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -16695,7 +17055,7 @@
       <c r="AMH14" s="2"/>
       <c r="AMI14" s="2"/>
     </row>
-    <row r="15" spans="1:1023" ht="14.1">
+    <row r="15" spans="1:1023">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -17722,7 +18082,7 @@
       <c r="AMH15" s="2"/>
       <c r="AMI15" s="2"/>
     </row>
-    <row r="16" spans="1:1023" ht="14.1">
+    <row r="16" spans="1:1023">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -18746,7 +19106,7 @@
       <c r="AMH16" s="2"/>
       <c r="AMI16" s="2"/>
     </row>
-    <row r="17" spans="1:1023" ht="14.1">
+    <row r="17" spans="1:1023">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -19773,7 +20133,7 @@
       <c r="AMH17" s="2"/>
       <c r="AMI17" s="2"/>
     </row>
-    <row r="18" spans="1:1023" ht="14.1">
+    <row r="18" spans="1:1023">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -20800,7 +21160,7 @@
       <c r="AMH18" s="2"/>
       <c r="AMI18" s="2"/>
     </row>
-    <row r="19" spans="1:1023" ht="14.1">
+    <row r="19" spans="1:1023">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -21827,7 +22187,7 @@
       <c r="AMH19" s="2"/>
       <c r="AMI19" s="2"/>
     </row>
-    <row r="20" spans="1:1023" ht="14.1">
+    <row r="20" spans="1:1023">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -22851,7 +23211,7 @@
       <c r="AMH20" s="2"/>
       <c r="AMI20" s="2"/>
     </row>
-    <row r="21" spans="1:1023" ht="14.1">
+    <row r="21" spans="1:1023">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -23880,7 +24240,7 @@
       <c r="AMH21" s="2"/>
       <c r="AMI21" s="2"/>
     </row>
-    <row r="22" spans="1:1023" ht="14.1">
+    <row r="22" spans="1:1023">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -24909,7 +25269,7 @@
       <c r="AMH22" s="2"/>
       <c r="AMI22" s="2"/>
     </row>
-    <row r="23" spans="1:1023" ht="14.1">
+    <row r="23" spans="1:1023">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -25938,7 +26298,7 @@
       <c r="AMH23" s="2"/>
       <c r="AMI23" s="2"/>
     </row>
-    <row r="24" spans="1:1023" ht="14.1">
+    <row r="24" spans="1:1023">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -26967,7 +27327,7 @@
       <c r="AMH24" s="2"/>
       <c r="AMI24" s="2"/>
     </row>
-    <row r="25" spans="1:1023" ht="14.1">
+    <row r="25" spans="1:1023">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -30072,16 +30432,16 @@
     </row>
     <row r="29" spans="1:1023">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
         <v>20</v>
@@ -30098,13 +30458,13 @@
     </row>
     <row r="30" spans="1:1023">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -30124,16 +30484,16 @@
     </row>
     <row r="31" spans="1:1023">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
         <v>27</v>
@@ -30149,16 +30509,7 @@
       </c>
     </row>
     <row r="32" spans="1:1023">
-      <c r="A32" t="s">
-        <v>100</v>
-      </c>
       <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32">
         <v>4</v>
       </c>
       <c r="E32" t="s">
@@ -30174,7 +30525,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="1:8">
       <c r="B33">
         <v>5</v>
       </c>
@@ -30191,7 +30542,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:8" s="5" customFormat="1">
+    <row r="34" spans="1:8" s="5" customFormat="1">
       <c r="B34">
         <v>6</v>
       </c>
@@ -30208,9 +30559,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>97</v>
+      </c>
       <c r="B35">
         <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
       </c>
       <c r="E35" t="s">
         <v>27</v>
@@ -30225,9 +30585,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="2:8">
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
       <c r="B36">
         <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
       </c>
       <c r="E36" t="s">
         <v>27</v>
@@ -30242,7 +30611,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="1:8">
       <c r="B37">
         <v>9</v>
       </c>
@@ -30259,7 +30628,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="1:8">
       <c r="B38">
         <v>10</v>
       </c>
@@ -30276,7 +30645,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="1:8">
       <c r="B39">
         <v>11</v>
       </c>
@@ -30293,7 +30662,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="1:8">
       <c r="B40">
         <v>12</v>
       </c>
@@ -30310,7 +30679,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="1:8">
       <c r="B41">
         <v>13</v>
       </c>
@@ -30327,7 +30696,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="1:8">
       <c r="B42">
         <v>14</v>
       </c>
@@ -30344,7 +30713,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="1:8">
       <c r="B43">
         <v>15</v>
       </c>
@@ -30361,7 +30730,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="1:8">
       <c r="B44">
         <v>16</v>
       </c>
@@ -30378,7 +30747,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="1:8">
       <c r="B45">
         <v>17</v>
       </c>
@@ -30395,7 +30764,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="1:8">
       <c r="B46">
         <v>18</v>
       </c>
@@ -30423,6 +30792,11 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -30434,18 +30808,18 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.09375" customWidth="1"/>
-    <col min="2" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.80859375" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="45.7109375" customWidth="1"/>
-    <col min="9" max="1024" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="4" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="6" max="6" width="45.75" customWidth="1"/>
+    <col min="7" max="7" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="45.75" customWidth="1"/>
+    <col min="9" max="1024" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -30459,7 +30833,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
@@ -30471,7 +30845,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="3" spans="1:8" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -30483,7 +30857,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
@@ -30495,7 +30869,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="5" spans="1:8" s="2" customFormat="1">
       <c r="A5" s="1"/>
       <c r="B5" s="7"/>
       <c r="C5" s="1"/>
@@ -30505,7 +30879,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
@@ -30519,7 +30893,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="7" spans="1:8" s="2" customFormat="1">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -30533,7 +30907,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="8" spans="1:8" s="2" customFormat="1">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -30547,7 +30921,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="9" spans="1:8" s="2" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -30561,7 +30935,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="10" spans="1:8" s="2" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -30575,7 +30949,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="11" spans="1:8" s="2" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -30589,7 +30963,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -30603,7 +30977,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="13" spans="1:8" s="2" customFormat="1">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -30617,7 +30991,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="14" spans="1:8" s="2" customFormat="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -30627,7 +31001,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="14.1">
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>88</v>
       </c>
@@ -30660,6 +31034,11 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -30671,18 +31050,18 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.09375" customWidth="1"/>
-    <col min="2" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.80859375" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="45.7109375" customWidth="1"/>
-    <col min="9" max="1024" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="4" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="6" max="6" width="45.75" customWidth="1"/>
+    <col min="7" max="7" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="45.75" customWidth="1"/>
+    <col min="9" max="1024" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -30696,7 +31075,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
@@ -30710,7 +31089,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="3" spans="1:8" s="2" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -30724,7 +31103,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
@@ -30738,7 +31117,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="5" spans="1:8" s="2" customFormat="1">
       <c r="A5" s="1"/>
       <c r="B5" s="7"/>
       <c r="C5" s="1"/>
@@ -30748,7 +31127,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
@@ -30762,7 +31141,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="7" spans="1:8" s="2" customFormat="1">
       <c r="A7" s="1" t="s">
         <v>81</v>
       </c>
@@ -30776,7 +31155,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="8" spans="1:8" s="2" customFormat="1">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -30790,7 +31169,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="9" spans="1:8" s="2" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>83</v>
       </c>
@@ -30804,7 +31183,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="10" spans="1:8" s="2" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -30818,7 +31197,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="11" spans="1:8" s="2" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -30832,7 +31211,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -30846,7 +31225,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="13" spans="1:8" s="2" customFormat="1">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -30860,7 +31239,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" ht="14.1">
+    <row r="14" spans="1:8" s="2" customFormat="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -30870,7 +31249,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="14.1">
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>88</v>
       </c>
@@ -30901,22 +31280,22 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
         <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -30924,22 +31303,22 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
         <v>98</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
         <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -30947,27 +31326,409 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C18" t="s">
         <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="4" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="6" max="6" width="45.75" customWidth="1"/>
+    <col min="7" max="7" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="45.75" customWidth="1"/>
+    <col min="9" max="1024" width="10.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="8">
+        <v>42642</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="8">
+        <v>42649</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="8">
+        <v>42649</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1">
+      <c r="A5" s="1"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1">
+      <c r="A8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1">
+      <c r="A9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1">
+      <c r="A10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>